<commit_message>
Correzione test di accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#LABICASRLXX/Labica_srl/fse2-connector/1.1.0/accreditamento-checklist_V8.1.3.xlsx
+++ b/GATEWAY/A1#111#LABICASRLXX/Labica_srl/fse2-connector/1.1.0/accreditamento-checklist_V8.1.3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\piero\Documenti\FSE\PR\it-fse-accreditamento\GATEWAY\A1#111#LABICASRLXX\Labica_srl\fse2-connector\1.1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\piero\Documenti\FSE\collaudo-validazione-20240410\GATEWAY\A1#111#LABICASRLXX\Labica_srl\fse2-connector\1.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="217">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -291,15 +291,6 @@
 </t>
   </si>
   <si>
-    <t>2024-04-10T12:50:14Z</t>
-  </si>
-  <si>
-    <t>8c8e16afbb600db9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.e1cbc413eb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
@@ -318,15 +309,6 @@
 </t>
   </si>
   <si>
-    <t>2024-04-10T12:50:34Z</t>
-  </si>
-  <si>
-    <t>74ba557de825f2b8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.0692ffef59^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT3</t>
   </si>
   <si>
@@ -336,15 +318,6 @@
 </t>
   </si>
   <si>
-    <t>2024-04-10T12:50:48Z</t>
-  </si>
-  <si>
-    <t>942c55aaac5f4cdd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d759054a6d79c3e5f58c855b80ace1fb6198ac06e560c98933861a00877d036b.87aa71e023^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT4</t>
   </si>
   <si>
@@ -354,15 +327,6 @@
 </t>
   </si>
   <si>
-    <t>2024-04-10T12:51:14Z</t>
-  </si>
-  <si>
-    <t>07ddb335e044adc1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d759054a6d79c3e5f58c855b80ace1fb6198ac06e560c98933861a00877d036b.f49a2caae6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT5</t>
   </si>
   <si>
@@ -370,15 +334,6 @@
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Il Documento CDA2 Laboratorio dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 5" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
 </t>
-  </si>
-  <si>
-    <t>2024-04-10T12:51:32Z</t>
-  </si>
-  <si>
-    <t>a00cbd33228d9b3c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.3db61240bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_LAB_KO</t>
@@ -430,15 +385,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-10T13:30:25Z</t>
-  </si>
-  <si>
-    <t>9a713f2f2ed24e43</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.38a2a28097^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>La sintassi del documento non è corretta</t>
   </si>
   <si>
@@ -449,15 +395,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-10T13:30:42Z</t>
-  </si>
-  <si>
-    <t>002ce2869d2421a2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.73341f7063^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il documento presenta degli errori nei contenuti</t>
   </si>
   <si>
@@ -468,15 +405,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-10T13:30:55Z</t>
-  </si>
-  <si>
-    <t>7802b90717ce0d70</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.7537e6730e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT9_KO</t>
   </si>
   <si>
@@ -484,15 +412,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-10T13:31:09Z</t>
-  </si>
-  <si>
-    <t>41e83dbc32098bce</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.8e570ade86^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT10_KO</t>
   </si>
   <si>
@@ -500,15 +419,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-10T13:31:20Z</t>
-  </si>
-  <si>
-    <t>63b776df4530b031</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.10dbb07f76^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT11_KO</t>
   </si>
   <si>
@@ -516,15 +426,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-10T13:31:36Z</t>
-  </si>
-  <si>
-    <t>67c81e2080e223de</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.c9afb1f816^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il documento ha dei contenuti non validi per il sistema FSE</t>
   </si>
   <si>
@@ -535,15 +436,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-10T13:35:19Z</t>
-  </si>
-  <si>
-    <t>3785aead3c4a50e6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.dc1786ab10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT13_KO</t>
   </si>
   <si>
@@ -551,15 +443,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-10T13:35:34Z</t>
-  </si>
-  <si>
-    <t>8c0368fa6b780095</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.e66688aa10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT14_KO</t>
   </si>
   <si>
@@ -567,12 +450,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>97b2283553725c55</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.18a147a7e0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT15_KO</t>
   </si>
   <si>
@@ -580,29 +457,11 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-10T13:36:04Z</t>
-  </si>
-  <si>
-    <t>d328db70a6d378a1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.095cc08dd1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT16_KO</t>
   </si>
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation"al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2024-04-10T13:36:17Z</t>
-  </si>
-  <si>
-    <t>d94237891bd6dbd8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d759054a6d79c3e5f58c855b80ace1fb6198ac06e560c98933861a00877d036b.8473544498^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT0</t>
@@ -614,15 +473,6 @@
 </t>
   </si>
   <si>
-    <t>2024-04-10T12:49:52Z</t>
-  </si>
-  <si>
-    <t>25c8a4d41e9869fc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.a1a891f736^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>ID TEST CASE OK</t>
   </si>
   <si>
@@ -823,6 +673,159 @@
   <si>
     <t>Il client che utilizza fse2-connector periodicamente interroga il sistema per ricevere lo stato dei referti inviati.
 Gli eventuali errori sono quindi gestiti nell'applicazione client che utilizza fse2-connector per interfacciarsi con il sistema FSE 2.0.</t>
+  </si>
+  <si>
+    <t>2024-04-19T13:56:13Z</t>
+  </si>
+  <si>
+    <t>7388c98fa5987072</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.051194da9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T13:56:36Z</t>
+  </si>
+  <si>
+    <t>d9a05cb33f9d132b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.712c021831^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T13:56:46Z</t>
+  </si>
+  <si>
+    <t>b948750b603fbc2c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.1cdf75e46b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T13:57:02Z</t>
+  </si>
+  <si>
+    <t>0dd652b108202e16</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d759054a6d79c3e5f58c855b80ace1fb6198ac06e560c98933861a00877d036b.a400808370^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T13:57:19Z</t>
+  </si>
+  <si>
+    <t>626b72ef07e4e358</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d759054a6d79c3e5f58c855b80ace1fb6198ac06e560c98933861a00877d036b.daf3c546a6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T13:57:39Z</t>
+  </si>
+  <si>
+    <t>4dd26b86e660fce8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.d075732252^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T13:57:56Z</t>
+  </si>
+  <si>
+    <t>606ed61500944fab</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.b45555a5aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:00:15Z</t>
+  </si>
+  <si>
+    <t>b71d8900d8e92734</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.50f48b8798^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:00:34Z</t>
+  </si>
+  <si>
+    <t>5e91c741156864d5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.96c0081328^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:00:48Z</t>
+  </si>
+  <si>
+    <t>00b24b15bd5d9065</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.9e0ec9db23^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:01:04Z</t>
+  </si>
+  <si>
+    <t>83352d193ebb28c6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.76888e8c59^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:01:15Z</t>
+  </si>
+  <si>
+    <t>03faa5e0eb6c7059</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.2d4b208606^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:01:26Z</t>
+  </si>
+  <si>
+    <t>0615c406db62ce2d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.8267c9d8cf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:01:39Z</t>
+  </si>
+  <si>
+    <t>c00119d0ad014bd7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.ba78a9e4ea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:01:50Z</t>
+  </si>
+  <si>
+    <t>86158adab41b9193</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.c950637c4a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:02:04Z</t>
+  </si>
+  <si>
+    <t>65498d1ea5406e1f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72b3386c1c02ddfd8ceda11bcdecab640ad935ffb58752f8beca7e6191d7f4da.73d942bde5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-04-19T14:02:16Z</t>
+  </si>
+  <si>
+    <t>54c6c2b4632b64cf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d759054a6d79c3e5f58c855b80ace1fb6198ac06e560c98933861a00877d036b.2d50ff63c6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1156,61 +1159,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1221,34 +1169,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1264,6 +1184,62 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3803,7 +3779,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,8 +3788,9 @@
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="63.85546875" customWidth="1"/>
-    <col min="5" max="5" width="104.85546875" customWidth="1"/>
-    <col min="6" max="9" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="104.85546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="9" width="33.140625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
     <col min="11" max="15" width="36.42578125" customWidth="1"/>
     <col min="16" max="16" width="56.28515625" customWidth="1"/>
@@ -3841,14 +3818,14 @@
       <c r="T1" s="14"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="55" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="55"/>
+      <c r="D2" s="26"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -3866,14 +3843,14 @@
       <c r="T2" s="14"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="57"/>
+      <c r="D3" s="28"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -3891,12 +3868,12 @@
       <c r="T3" s="14"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="57" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="57"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="1"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -3915,12 +3892,12 @@
       <c r="T4" s="14"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="57" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="57"/>
+      <c r="D5" s="28"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -3938,8 +3915,8 @@
       <c r="T5" s="14"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="53"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="16"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -4056,264 +4033,264 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20">
+    <row r="10" spans="1:20" s="38" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29">
         <v>1</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G10" s="23" t="s">
+      <c r="F10" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="J10" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="R10" s="35"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="25" t="s">
+    </row>
+    <row r="11" spans="1:20" s="38" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29">
+        <v>2</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25" t="s">
+      <c r="E11" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="R10" s="26"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="28" t="s">
+      <c r="F11" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="38" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29">
+        <v>3</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="30" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
-        <v>2</v>
-      </c>
-      <c r="B11" s="21" t="s">
+      <c r="E12" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="38" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29">
+        <v>4</v>
+      </c>
+      <c r="B13" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C13" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="22" t="s">
+      <c r="D13" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="E13" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="F13" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="38" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29">
+        <v>5</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="E14" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="J11" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20">
-        <v>3</v>
-      </c>
-      <c r="B12" s="21" t="s">
+      <c r="F14" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="38" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29">
+        <v>28</v>
+      </c>
+      <c r="B15" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C15" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D15" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E15" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="K15" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="37" t="s">
         <v>67</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20">
-        <v>4</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20">
-        <v>5</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20">
-        <v>28</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="K15" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="28" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="38" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4327,20 +4304,20 @@
         <v>49</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
       <c r="I16" s="33"/>
       <c r="J16" s="34" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
@@ -4351,7 +4328,7 @@
       <c r="R16" s="35"/>
       <c r="S16" s="36"/>
       <c r="T16" s="37" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="38" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4365,753 +4342,753 @@
         <v>49</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>
       <c r="J17" s="34" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K17" s="34"/>
       <c r="L17" s="34" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="M17" s="34" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="N17" s="34"/>
       <c r="O17" s="34" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P17" s="34" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="Q17" s="34"/>
       <c r="R17" s="35" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="S17" s="36"/>
       <c r="T17" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29">
+        <v>52</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M18" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O18" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29">
+        <v>53</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M19" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O19" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P19" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="29">
+        <v>54</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O20" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P20" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="29">
+        <v>55</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="30" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20">
+      <c r="E21" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="J21" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="K21" s="34"/>
+      <c r="L21" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O21" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P21" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="29">
+        <v>56</v>
+      </c>
+      <c r="B22" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C22" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D22" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="H22" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="I22" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M22" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N22" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O22" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="29">
+        <v>57</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="I23" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="J23" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M23" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N23" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="O23" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P23" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29">
+        <v>58</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E24" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G18" s="24" t="s">
+      <c r="F24" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="H24" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M24" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N24" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O24" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P24" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="29">
+        <v>59</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="E25" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="F25" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="I25" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="J25" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M25" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N25" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O25" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P25" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="29">
+        <v>60</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N18" s="25" t="s">
+      <c r="E26" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="O18" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P18" s="25" t="s">
+      <c r="F26" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M26" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N26" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O26" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P26" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="29">
+        <v>61</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M27" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N27" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O27" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P27" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" s="38" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="29">
+        <v>62</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="H28" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20">
-        <v>53</v>
-      </c>
-      <c r="B19" s="21" t="s">
+      <c r="I28" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M28" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O28" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q28" s="34"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" s="48" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="39">
+        <v>191</v>
+      </c>
+      <c r="B29" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C29" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M19" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N19" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O19" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P19" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20">
-        <v>54</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="J20" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M20" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N20" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O20" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P20" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20">
-        <v>55</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N21" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O21" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P21" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20">
-        <v>56</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N22" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O22" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P22" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20">
-        <v>57</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="F23" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="J23" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M23" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N23" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="O23" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P23" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="27"/>
-      <c r="T23" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20">
-        <v>58</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F24" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="J24" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M24" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N24" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O24" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P24" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20">
-        <v>59</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="F25" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="J25" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M25" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N25" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="O25" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P25" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="27"/>
-      <c r="T25" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20">
-        <v>60</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="F26" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="H26" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="J26" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M26" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N26" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O26" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P26" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="27"/>
-      <c r="T26" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20">
-        <v>61</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="F27" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="J27" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M27" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N27" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O27" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P27" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="20">
-        <v>62</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="F28" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="J28" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M28" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N28" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="O28" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P28" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" s="52" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="43">
-        <v>191</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="E29" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="F29" s="46"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
+      <c r="D29" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="F29" s="42"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
       <c r="J29" s="34" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="L29" s="34"/>
       <c r="M29" s="34"/>
-      <c r="N29" s="48"/>
+      <c r="N29" s="44"/>
       <c r="O29" s="34"/>
-      <c r="P29" s="48"/>
+      <c r="P29" s="44"/>
       <c r="Q29" s="34"/>
-      <c r="R29" s="49"/>
-      <c r="S29" s="50"/>
-      <c r="T29" s="51" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="20">
+      <c r="R29" s="45"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" s="38" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="29">
         <v>368</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" s="23">
-        <v>45392</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="H30" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="J30" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" s="52" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A31" s="43">
+      <c r="D30" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="32">
+        <v>45401</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="J30" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="35"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" s="48" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A31" s="39">
         <v>376</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="44" t="s">
-        <v>212</v>
-      </c>
-      <c r="E31" s="45" t="s">
-        <v>213</v>
-      </c>
-      <c r="F31" s="46"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
+      <c r="D31" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="F31" s="42"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
       <c r="J31" s="34" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="34"/>
       <c r="N31" s="34"/>
       <c r="O31" s="34"/>
-      <c r="P31" s="48"/>
+      <c r="P31" s="44"/>
       <c r="Q31" s="34"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="50"/>
-      <c r="T31" s="51" t="s">
-        <v>57</v>
+      <c r="R31" s="45"/>
+      <c r="S31" s="46"/>
+      <c r="T31" s="47" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10184,10 +10161,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10195,125 +10172,125 @@
         <v>49</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>155</v>
+        <v>103</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>158</v>
+        <v>103</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>161</v>
+        <v>103</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>164</v>
+        <v>103</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>167</v>
+        <v>103</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>170</v>
+        <v>103</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>173</v>
+        <v>103</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>176</v>
+        <v>103</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>179</v>
+        <v>103</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10321,111 +10298,111 @@
         <v>49</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C11" s="39">
+        <v>130</v>
+      </c>
+      <c r="C11" s="20">
         <v>192</v>
       </c>
-      <c r="D11" s="39" t="s">
-        <v>181</v>
+      <c r="D11" s="20" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" s="39">
+        <v>130</v>
+      </c>
+      <c r="C12" s="20">
         <v>208</v>
       </c>
-      <c r="D12" s="39" t="s">
-        <v>182</v>
+      <c r="D12" s="20" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" s="39">
+        <v>130</v>
+      </c>
+      <c r="C13" s="20">
         <v>224</v>
       </c>
-      <c r="D13" s="40" t="s">
-        <v>183</v>
+      <c r="D13" s="21" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C14" s="39">
+        <v>130</v>
+      </c>
+      <c r="C14" s="20">
         <v>240</v>
       </c>
-      <c r="D14" s="39" t="s">
-        <v>184</v>
+      <c r="D14" s="20" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" s="39">
+        <v>130</v>
+      </c>
+      <c r="C15" s="20">
         <v>256</v>
       </c>
-      <c r="D15" s="40" t="s">
-        <v>185</v>
+      <c r="D15" s="21" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C16" s="39">
+        <v>130</v>
+      </c>
+      <c r="C16" s="20">
         <v>272</v>
       </c>
-      <c r="D16" s="40" t="s">
-        <v>186</v>
+      <c r="D16" s="21" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C17" s="39">
+        <v>130</v>
+      </c>
+      <c r="C17" s="20">
         <v>288</v>
       </c>
-      <c r="D17" s="40" t="s">
-        <v>187</v>
+      <c r="D17" s="21" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C18" s="39">
+        <v>130</v>
+      </c>
+      <c r="C18" s="20">
         <v>304</v>
       </c>
-      <c r="D18" s="40" t="s">
-        <v>188</v>
+      <c r="D18" s="21" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10433,111 +10410,111 @@
         <v>49</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C19" s="39">
+        <v>139</v>
+      </c>
+      <c r="C19" s="20">
         <v>193</v>
       </c>
-      <c r="D19" s="39" t="s">
-        <v>190</v>
+      <c r="D19" s="20" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C20" s="39">
+        <v>139</v>
+      </c>
+      <c r="C20" s="20">
         <v>209</v>
       </c>
-      <c r="D20" s="39" t="s">
-        <v>191</v>
+      <c r="D20" s="20" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C21" s="39">
+        <v>139</v>
+      </c>
+      <c r="C21" s="20">
         <v>225</v>
       </c>
-      <c r="D21" s="40" t="s">
-        <v>192</v>
+      <c r="D21" s="21" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C22" s="39">
+        <v>139</v>
+      </c>
+      <c r="C22" s="20">
         <v>241</v>
       </c>
-      <c r="D22" s="39" t="s">
-        <v>193</v>
+      <c r="D22" s="20" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23" s="39">
+        <v>139</v>
+      </c>
+      <c r="C23" s="20">
         <v>257</v>
       </c>
-      <c r="D23" s="40" t="s">
-        <v>194</v>
+      <c r="D23" s="21" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C24" s="39">
+        <v>139</v>
+      </c>
+      <c r="C24" s="20">
         <v>273</v>
       </c>
-      <c r="D24" s="40" t="s">
-        <v>195</v>
+      <c r="D24" s="21" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C25" s="39">
+        <v>139</v>
+      </c>
+      <c r="C25" s="20">
         <v>289</v>
       </c>
-      <c r="D25" s="40" t="s">
-        <v>196</v>
+      <c r="D25" s="21" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C26" s="39">
+        <v>139</v>
+      </c>
+      <c r="C26" s="20">
         <v>305</v>
       </c>
-      <c r="D26" s="40" t="s">
-        <v>197</v>
+      <c r="D26" s="21" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10545,111 +10522,111 @@
         <v>49</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C27" s="39">
+        <v>148</v>
+      </c>
+      <c r="C27" s="20">
         <v>194</v>
       </c>
-      <c r="D27" s="39" t="s">
-        <v>199</v>
+      <c r="D27" s="20" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C28" s="39">
+        <v>148</v>
+      </c>
+      <c r="C28" s="20">
         <v>210</v>
       </c>
-      <c r="D28" s="39" t="s">
-        <v>200</v>
+      <c r="D28" s="20" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C29" s="39">
+        <v>148</v>
+      </c>
+      <c r="C29" s="20">
         <v>226</v>
       </c>
-      <c r="D29" s="41" t="s">
-        <v>201</v>
+      <c r="D29" s="22" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C30" s="39">
+        <v>148</v>
+      </c>
+      <c r="C30" s="20">
         <v>242</v>
       </c>
-      <c r="D30" s="39" t="s">
-        <v>202</v>
+      <c r="D30" s="20" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C31" s="39">
+        <v>148</v>
+      </c>
+      <c r="C31" s="20">
         <v>258</v>
       </c>
-      <c r="D31" s="40" t="s">
-        <v>203</v>
+      <c r="D31" s="21" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C32" s="39">
+        <v>148</v>
+      </c>
+      <c r="C32" s="20">
         <v>274</v>
       </c>
-      <c r="D32" s="40" t="s">
-        <v>204</v>
+      <c r="D32" s="21" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C33" s="39">
+        <v>148</v>
+      </c>
+      <c r="C33" s="20">
         <v>290</v>
       </c>
-      <c r="D33" s="40" t="s">
-        <v>205</v>
+      <c r="D33" s="21" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C34" s="39">
+        <v>148</v>
+      </c>
+      <c r="C34" s="20">
         <v>306</v>
       </c>
-      <c r="D34" s="40" t="s">
-        <v>206</v>
+      <c r="D34" s="21" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10657,110 +10634,110 @@
         <v>49</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C35" s="39">
+        <v>157</v>
+      </c>
+      <c r="C35" s="20">
         <v>195</v>
       </c>
-      <c r="D35" s="39">
+      <c r="D35" s="20">
         <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C36" s="39">
+        <v>157</v>
+      </c>
+      <c r="C36" s="20">
         <v>211</v>
       </c>
-      <c r="D36" s="39">
+      <c r="D36" s="20">
         <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C37" s="39">
+        <v>157</v>
+      </c>
+      <c r="C37" s="20">
         <v>227</v>
       </c>
-      <c r="D37" s="40">
+      <c r="D37" s="21">
         <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C38" s="39">
+        <v>157</v>
+      </c>
+      <c r="C38" s="20">
         <v>243</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="20">
         <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C39" s="39">
+        <v>157</v>
+      </c>
+      <c r="C39" s="20">
         <v>259</v>
       </c>
-      <c r="D39" s="40">
+      <c r="D39" s="21">
         <v>268</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C40" s="39">
+        <v>157</v>
+      </c>
+      <c r="C40" s="20">
         <v>275</v>
       </c>
-      <c r="D40" s="40">
+      <c r="D40" s="21">
         <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C41" s="39">
+        <v>157</v>
+      </c>
+      <c r="C41" s="20">
         <v>291</v>
       </c>
-      <c r="D41" s="40">
+      <c r="D41" s="21">
         <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C42" s="39">
+        <v>157</v>
+      </c>
+      <c r="C42" s="20">
         <v>307</v>
       </c>
-      <c r="D42" s="40">
+      <c r="D42" s="21">
         <v>316</v>
       </c>
     </row>
@@ -10769,110 +10746,110 @@
         <v>49</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C43" s="39">
+        <v>158</v>
+      </c>
+      <c r="C43" s="20">
         <v>196</v>
       </c>
-      <c r="D43" s="39">
+      <c r="D43" s="20">
         <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C44" s="39">
+        <v>158</v>
+      </c>
+      <c r="C44" s="20">
         <v>212</v>
       </c>
-      <c r="D44" s="39">
+      <c r="D44" s="20">
         <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C45" s="39">
+        <v>158</v>
+      </c>
+      <c r="C45" s="20">
         <v>228</v>
       </c>
-      <c r="D45" s="40">
+      <c r="D45" s="21">
         <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C46" s="39">
+        <v>158</v>
+      </c>
+      <c r="C46" s="20">
         <v>244</v>
       </c>
-      <c r="D46" s="39">
+      <c r="D46" s="20">
         <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C47" s="39">
+        <v>158</v>
+      </c>
+      <c r="C47" s="20">
         <v>260</v>
       </c>
-      <c r="D47" s="40">
+      <c r="D47" s="21">
         <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C48" s="39">
+        <v>158</v>
+      </c>
+      <c r="C48" s="20">
         <v>276</v>
       </c>
-      <c r="D48" s="40">
+      <c r="D48" s="21">
         <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C49" s="39">
+        <v>158</v>
+      </c>
+      <c r="C49" s="20">
         <v>292</v>
       </c>
-      <c r="D49" s="40">
+      <c r="D49" s="21">
         <v>303</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C50" s="39">
+        <v>158</v>
+      </c>
+      <c r="C50" s="20">
         <v>308</v>
       </c>
-      <c r="D50" s="40">
+      <c r="D50" s="21">
         <v>319</v>
       </c>
     </row>
@@ -11848,32 +11825,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>55</v>
+      <c r="A2" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>80</v>
+      <c r="A3" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
     </row>
     <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>